<commit_message>
test response message and status code for api testing
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/connection/connection_page.xlsx
+++ b/apps/features/backlog/android/connection/connection_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\connection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92421D8-ADA0-4A42-B80B-C8F8FB9014B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54CBEE4-FBFB-428F-837F-055C4A201B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="141">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>1. VPN app is installed and open.</t>
-  </si>
-  <si>
-    <t>try to reconnection after disconnection</t>
   </si>
   <si>
     <t>Scenario : Connection Page</t>
@@ -194,9 +191,6 @@
   </si>
   <si>
     <t>should be changed</t>
-  </si>
-  <si>
-    <t>connect with vpn server</t>
   </si>
   <si>
     <t>will disconnect the vpn</t>
@@ -489,16 +483,6 @@
   <si>
     <t>1. go to playstore and install symlexvpn in the mobile.
 2. open the installed symlexvpn application.
-3. Login with proper credentials
-4. turn on connection button
-5. disconnect from the vpn server.
-6.verify that the vpn connection is disconnected.
-7.click on the "connect" button.
-8.verify that the vpn connection is successfully reestablished.</t>
-  </si>
-  <si>
-    <t>1. go to playstore and install symlexvpn in the mobile.
-2. open the installed symlexvpn application.
 3. login with proper credentials
 4. navigate to the VPN connection page.
 5. select a server from the available list
@@ -630,6 +614,35 @@
 4. navigate to the vpn connection page.
 5. click on "connect" button
 6. goto browser , check DNS leak on ip-score website</t>
+  </si>
+  <si>
+    <t>should connect with vpn server</t>
+  </si>
+  <si>
+    <t>try to reconnection with another server while connecting to other server</t>
+  </si>
+  <si>
+    <t>1. go to microsoftstore and install symlexvpn in the windows.
+2. open the installed symlexvpn application.
+3. Login with proper credentials
+4. turn on connection button
+5. try to reconnection with another server while connecting to other server 
+7. verify that the vpn connection is successfully reestablished.</t>
+  </si>
+  <si>
+    <t>check if the local ip is changing in the device connection page after connecting to server</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the iphone.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page.
+5. local ip will show in the connection page
+6. connect to server, ip will change to that server ip
+7. disconnect the server, ip will change into the local ip</t>
+  </si>
+  <si>
+    <t>TC_SYM_AC_033</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1614,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G33" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G34" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1819,8 +1832,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1837,7 +1850,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1940,19 +1953,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>7</v>
@@ -1982,19 +1995,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="3"/>
@@ -2022,19 +2035,19 @@
         <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="3"/>
@@ -2062,19 +2075,19 @@
         <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="3"/>
@@ -2102,19 +2115,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
@@ -2142,19 +2155,19 @@
         <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="F9" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4"/>
@@ -2182,19 +2195,19 @@
         <v>16</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4"/>
@@ -2222,19 +2235,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="1"/>
@@ -2262,19 +2275,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="1"/>
@@ -2302,19 +2315,19 @@
         <v>19</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
@@ -2342,19 +2355,19 @@
         <v>20</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
@@ -2382,19 +2395,19 @@
         <v>21</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="F15" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="1"/>
@@ -2422,19 +2435,19 @@
         <v>22</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>24</v>
+      <c r="C16" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="1"/>
@@ -2457,24 +2470,24 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="1"/>
@@ -2499,22 +2512,22 @@
     </row>
     <row r="18" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="1"/>
@@ -2539,22 +2552,22 @@
     </row>
     <row r="19" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="1"/>
@@ -2579,22 +2592,22 @@
     </row>
     <row r="20" spans="1:26" ht="143.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="1"/>
@@ -2619,22 +2632,22 @@
     </row>
     <row r="21" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="1"/>
@@ -2659,22 +2672,22 @@
     </row>
     <row r="22" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="1"/>
@@ -2699,22 +2712,22 @@
     </row>
     <row r="23" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="1"/>
@@ -2739,22 +2752,22 @@
     </row>
     <row r="24" spans="1:26" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="1"/>
@@ -2779,22 +2792,22 @@
     </row>
     <row r="25" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="1"/>
@@ -2819,22 +2832,22 @@
     </row>
     <row r="26" spans="1:26" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="F26" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="1"/>
@@ -2859,22 +2872,22 @@
     </row>
     <row r="27" spans="1:26" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="F27" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="1"/>
@@ -2899,22 +2912,22 @@
     </row>
     <row r="28" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="1"/>
@@ -2939,22 +2952,22 @@
     </row>
     <row r="29" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>66</v>
+      <c r="D29" s="6" t="s">
+        <v>130</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="F29" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="1"/>
@@ -2979,22 +2992,22 @@
     </row>
     <row r="30" spans="1:26" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="1"/>
@@ -3019,22 +3032,22 @@
     </row>
     <row r="31" spans="1:26" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>54</v>
-      </c>
       <c r="F31" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="1"/>
@@ -3059,22 +3072,22 @@
     </row>
     <row r="32" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="F32" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="1"/>
@@ -3099,22 +3112,22 @@
     </row>
     <row r="33" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="1"/>
@@ -3138,13 +3151,25 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="A34" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="13"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -29931,7 +29956,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F33" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F34" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>